<commit_message>
Alleged final commit. Changed title of group1_plot
</commit_message>
<xml_diff>
--- a/data/group_3_data.xlsx
+++ b/data/group_3_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Y3948024/figure_and_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{974D40B9-6212-434C-84D0-F7071F5821B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E310BF2-B30B-BA4B-841F-E30768ED944E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="1000" windowWidth="26420" windowHeight="15840" xr2:uid="{C870EA4A-6BEE-A045-B045-35254FC4C783}"/>
+    <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="15980" xr2:uid="{C870EA4A-6BEE-A045-B045-35254FC4C783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,6 +486,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>5500000</v>
+      </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
@@ -497,6 +500,9 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>7200000</v>
+      </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
@@ -508,6 +514,9 @@
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>5300000</v>
+      </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
@@ -518,6 +527,9 @@
       </c>
       <c r="B5">
         <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3500000</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -530,6 +542,9 @@
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="C6">
+        <v>38000000</v>
+      </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -541,6 +556,9 @@
       <c r="B7">
         <v>2</v>
       </c>
+      <c r="C7">
+        <v>39000000</v>
+      </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
@@ -552,6 +570,9 @@
       <c r="B8">
         <v>3</v>
       </c>
+      <c r="C8">
+        <v>35000000</v>
+      </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
@@ -563,6 +584,9 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="C9">
+        <v>43000000</v>
+      </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
@@ -574,6 +598,9 @@
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10">
+        <v>13000000</v>
+      </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
@@ -585,6 +612,9 @@
       <c r="B11">
         <v>2</v>
       </c>
+      <c r="C11">
+        <v>17000000</v>
+      </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
@@ -596,6 +626,9 @@
       <c r="B12">
         <v>3</v>
       </c>
+      <c r="C12">
+        <v>12000000</v>
+      </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
@@ -607,6 +640,9 @@
       <c r="B13">
         <v>4</v>
       </c>
+      <c r="C13">
+        <v>16000000</v>
+      </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -618,6 +654,9 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="C14">
+        <v>690000</v>
+      </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
@@ -629,6 +668,9 @@
       <c r="B15">
         <v>2</v>
       </c>
+      <c r="C15">
+        <v>770000</v>
+      </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
@@ -640,6 +682,9 @@
       <c r="B16">
         <v>3</v>
       </c>
+      <c r="C16">
+        <v>710000</v>
+      </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
@@ -651,6 +696,9 @@
       <c r="B17">
         <v>4</v>
       </c>
+      <c r="C17">
+        <v>810000</v>
+      </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
@@ -662,6 +710,9 @@
       <c r="B18">
         <v>1</v>
       </c>
+      <c r="C18">
+        <v>470000</v>
+      </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -673,6 +724,9 @@
       <c r="B19">
         <v>2</v>
       </c>
+      <c r="C19">
+        <v>520000</v>
+      </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
@@ -684,6 +738,9 @@
       <c r="B20">
         <v>3</v>
       </c>
+      <c r="C20">
+        <v>560000</v>
+      </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
@@ -695,6 +752,9 @@
       <c r="B21">
         <v>4</v>
       </c>
+      <c r="C21">
+        <v>420000</v>
+      </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
@@ -706,6 +766,9 @@
       <c r="B22">
         <v>1</v>
       </c>
+      <c r="C22">
+        <v>410000</v>
+      </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
@@ -717,6 +780,9 @@
       <c r="B23">
         <v>2</v>
       </c>
+      <c r="C23">
+        <v>510000</v>
+      </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
@@ -728,6 +794,9 @@
       <c r="B24">
         <v>3</v>
       </c>
+      <c r="C24">
+        <v>430000</v>
+      </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
@@ -739,6 +808,9 @@
       <c r="B25">
         <v>4</v>
       </c>
+      <c r="C25">
+        <v>410000</v>
+      </c>
       <c r="D25" t="s">
         <v>13</v>
       </c>
@@ -750,6 +822,9 @@
       <c r="B26">
         <v>1</v>
       </c>
+      <c r="C26">
+        <v>4600000</v>
+      </c>
       <c r="D26" t="s">
         <v>13</v>
       </c>
@@ -761,6 +836,9 @@
       <c r="B27">
         <v>2</v>
       </c>
+      <c r="C27">
+        <v>2800000</v>
+      </c>
       <c r="D27" t="s">
         <v>13</v>
       </c>
@@ -772,6 +850,9 @@
       <c r="B28">
         <v>3</v>
       </c>
+      <c r="C28">
+        <v>3500000</v>
+      </c>
       <c r="D28" t="s">
         <v>13</v>
       </c>
@@ -783,6 +864,9 @@
       <c r="B29">
         <v>4</v>
       </c>
+      <c r="C29">
+        <v>4000000</v>
+      </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
@@ -794,6 +878,9 @@
       <c r="B30">
         <v>1</v>
       </c>
+      <c r="C30">
+        <v>3700000</v>
+      </c>
       <c r="D30" t="s">
         <v>13</v>
       </c>
@@ -805,6 +892,9 @@
       <c r="B31">
         <v>2</v>
       </c>
+      <c r="C31">
+        <v>5300000</v>
+      </c>
       <c r="D31" t="s">
         <v>13</v>
       </c>
@@ -816,6 +906,9 @@
       <c r="B32">
         <v>3</v>
       </c>
+      <c r="C32">
+        <v>5200000</v>
+      </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
@@ -826,6 +919,9 @@
       </c>
       <c r="B33">
         <v>4</v>
+      </c>
+      <c r="C33">
+        <v>4000000</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Group 3 plot almost finished
</commit_message>
<xml_diff>
--- a/data/group_3_data.xlsx
+++ b/data/group_3_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Y3948024/figure_and_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E310BF2-B30B-BA4B-841F-E30768ED944E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42363878-439A-3E42-A67E-FDA9706DDC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="15980" xr2:uid="{C870EA4A-6BEE-A045-B045-35254FC4C783}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Plate</t>
   </si>
   <si>
-    <t>Spot</t>
-  </si>
-  <si>
     <t>cfu_count_undiluted</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Without hexadecane</t>
+  </si>
+  <si>
+    <t>spot</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,18 +470,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -490,12 +490,12 @@
         <v>5500000</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -504,12 +504,12 @@
         <v>7200000</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -518,12 +518,12 @@
         <v>5300000</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -532,12 +532,12 @@
         <v>3500000</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -546,12 +546,12 @@
         <v>38000000</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -560,12 +560,12 @@
         <v>39000000</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -574,12 +574,12 @@
         <v>35000000</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -588,12 +588,12 @@
         <v>43000000</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -602,12 +602,12 @@
         <v>13000000</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -616,12 +616,12 @@
         <v>17000000</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -630,12 +630,12 @@
         <v>12000000</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -644,12 +644,12 @@
         <v>16000000</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -658,12 +658,12 @@
         <v>690000</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -672,12 +672,12 @@
         <v>770000</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -686,12 +686,12 @@
         <v>710000</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -700,12 +700,12 @@
         <v>810000</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -714,12 +714,12 @@
         <v>470000</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -728,12 +728,12 @@
         <v>520000</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -742,12 +742,12 @@
         <v>560000</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -756,12 +756,12 @@
         <v>420000</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -770,12 +770,12 @@
         <v>410000</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -784,12 +784,12 @@
         <v>510000</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -798,12 +798,12 @@
         <v>430000</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -812,12 +812,12 @@
         <v>410000</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -826,12 +826,12 @@
         <v>4600000</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -840,12 +840,12 @@
         <v>2800000</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -854,12 +854,12 @@
         <v>3500000</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -868,12 +868,12 @@
         <v>4000000</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -882,12 +882,12 @@
         <v>3700000</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -896,12 +896,12 @@
         <v>5300000</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -910,12 +910,12 @@
         <v>5200000</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -924,7 +924,7 @@
         <v>4000000</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Group 3 plot commit
</commit_message>
<xml_diff>
--- a/data/group_3_data.xlsx
+++ b/data/group_3_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Y3948024/figure_and_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42363878-439A-3E42-A67E-FDA9706DDC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3098004-7D87-7E4D-A16C-E570456666F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="15980" xr2:uid="{C870EA4A-6BEE-A045-B045-35254FC4C783}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>5500000</v>
+        <v>1100000</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>7200000</v>
+        <v>1440000</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>5300000</v>
+        <v>1060000</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>3500000</v>
+        <v>700000</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -543,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>38000000</v>
+        <v>7600000</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -557,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>39000000</v>
+        <v>7800000</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>35000000</v>
+        <v>7000000</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -585,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>43000000</v>
+        <v>8600000</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -599,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>13000000</v>
+        <v>2600000</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>17000000</v>
+        <v>3400000</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>12000000</v>
+        <v>2400000</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -641,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>16000000</v>
+        <v>3200000</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -655,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>690000</v>
+        <v>138000</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -669,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>770000</v>
+        <v>154000</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -683,7 +683,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>710000</v>
+        <v>142000</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -697,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>810000</v>
+        <v>162000</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -711,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>470000</v>
+        <v>94000</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>520000</v>
+        <v>104000</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -739,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>560000</v>
+        <v>112000</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <v>420000</v>
+        <v>84000</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>410000</v>
+        <v>82000</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -781,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>510000</v>
+        <v>102000</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -795,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>430000</v>
+        <v>86000</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>410000</v>
+        <v>82000</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>4600000</v>
+        <v>920000</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <v>2800000</v>
+        <v>560000</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -851,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>3500000</v>
+        <v>700000</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -865,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>4000000</v>
+        <v>800000</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -879,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>3700000</v>
+        <v>740000</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="C31">
-        <v>5300000</v>
+        <v>1060000</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -907,7 +907,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>5200000</v>
+        <v>1040000</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -921,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="C33">
-        <v>4000000</v>
+        <v>800000</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>

</xml_diff>